<commit_message>
https://jira.aplana.com/browse/SBRFNDFL-3844 Патч БД 2.2.1
</commit_message>
<xml_diff>
--- a/database/database-2.2.1/templates/data/ndfl/consolidated_rnu_ndfl/v2016/rnu_ndfl_person_all_db.xlsx
+++ b/database/database-2.2.1/templates/data/ndfl/consolidated_rnu_ndfl/v2016/rnu_ndfl_person_all_db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="28755" windowHeight="13875" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="28755" windowHeight="13875"/>
   </bookViews>
   <sheets>
     <sheet name="Заголовок" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,6 @@
     <t>Подразделение</t>
   </si>
   <si>
-    <t>Регистр налогового учета на доходы физических лиц</t>
-  </si>
-  <si>
     <t>за</t>
   </si>
   <si>
@@ -226,50 +223,8 @@
 (%)</t>
   </si>
   <si>
-    <t>НДФЛ.Расчет.
-Дата</t>
-  </si>
-  <si>
-    <t>НДФЛ.Расчет.
-Сумма.
-Исчисленный</t>
-  </si>
-  <si>
-    <t>НДФЛ.Расчет.
-Сумма.
-Удержанный</t>
-  </si>
-  <si>
-    <t>НДФЛ.Расчет.
-Сумма.
-Не удержанный</t>
-  </si>
-  <si>
-    <t>НДФЛ.Расчет.
-Сумма.Излишне удержанный</t>
-  </si>
-  <si>
-    <t>НДФЛ.Расчет.
-Сумма.Возвращенный налогоплательщику</t>
-  </si>
-  <si>
     <t>Перечисление в бюджет.
 Срок</t>
-  </si>
-  <si>
-    <t>Перечисление в бюджет.
-Платежное поручение.
-Дата</t>
-  </si>
-  <si>
-    <t>Перечисление в бюджет.
-Платежное поручение.
-Номер</t>
-  </si>
-  <si>
-    <t>Перечисление в бюджет.
-Платежное поручение.
-Сумма</t>
   </si>
   <si>
     <t>Код вычета</t>
@@ -358,6 +313,51 @@
   </si>
   <si>
     <t>Применение вычета.Сумма применённого вычета с начала налогового периода</t>
+  </si>
+  <si>
+    <t>НДФЛ.Расчёт.
+Дата</t>
+  </si>
+  <si>
+    <t>НДФЛ.Расчёт.
+Сумма.
+Исчисленный</t>
+  </si>
+  <si>
+    <t>НДФЛ.Расчёт.
+Сумма.
+Удержанный</t>
+  </si>
+  <si>
+    <t>НДФЛ.Расчёт.
+Сумма.
+Не удержанный</t>
+  </si>
+  <si>
+    <t>НДФЛ.Расчёт.
+Сумма.Излишне удержанный</t>
+  </si>
+  <si>
+    <t>Перечисление в бюджет.
+Платёжное поручение.
+Дата</t>
+  </si>
+  <si>
+    <t>Перечисление в бюджет.
+Платёжное поручение.
+Номер</t>
+  </si>
+  <si>
+    <t>Перечисление в бюджет.
+Платёжное поручение.
+Сумма</t>
+  </si>
+  <si>
+    <t>НДФЛ.Расчёт.
+Сумма.Возвращённый налогоплательщику</t>
+  </si>
+  <si>
+    <t>Регистр налогового учёта на доходы физических лиц</t>
   </si>
 </sst>
 </file>
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -764,17 +764,17 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:W3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -818,67 +818,67 @@
   <sheetData>
     <row r="2" spans="2:23">
       <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="W2" s="3">
         <v>22</v>
@@ -886,70 +886,70 @@
     </row>
     <row r="3" spans="2:23" ht="31.5">
       <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="V3" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="W3" s="3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -962,7 +962,7 @@
   <dimension ref="A2:Y3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Y3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -993,151 +993,151 @@
     <row r="2" spans="1:25">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="W2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="42">
       <c r="A3" s="4"/>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="W3" s="3" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1167,103 +1167,103 @@
     <row r="2" spans="1:17">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="52.5">
       <c r="A3" s="4"/>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1276,7 +1276,7 @@
   <dimension ref="A2:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1293,49 +1293,49 @@
     <row r="2" spans="1:8">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="52.5">
       <c r="A3" s="4"/>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>